<commit_message>
#983 , #984 #985, #986 , #987 결함 해결
</commit_message>
<xml_diff>
--- a/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스_05_penta.xlsx
+++ b/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스_05_penta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="346">
   <si>
     <t>TestCase ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -451,10 +451,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>결함 존재</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>UC001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -765,6 +761,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Pass</t>
+  </si>
+  <si>
     <t>UC004</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -801,10 +800,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>입력값 그대로 출력됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>과목 등록시 시간 구분 기능에 대한 에러
 검출 (시작 시간이 종료 시간보다 더 이후의 시간일 경우)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -834,14 +829,6 @@
   </si>
   <si>
     <t>1.오류팝업창 이외의 버튼들을 클릭</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>디폴트 값인        '과목명'이라고 출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>디폴트 값인        '담당 교수명' 이라고 출력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1504,7 +1491,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>결함 존재</t>
+    <t>#983</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#985</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#984</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#986</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#987</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2364,8 +2367,8 @@
   <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2401,7 +2404,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2409,7 +2412,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2449,7 +2452,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>20</v>
@@ -2461,7 +2464,7 @@
         <v>97</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H8" s="21" t="s">
         <v>21</v>
@@ -2470,7 +2473,7 @@
         <v>22</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K8" s="1"/>
     </row>
@@ -2479,31 +2482,31 @@
         <v>95</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>96</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>98</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H9" s="21" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>100</v>
+        <v>341</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -2511,19 +2514,19 @@
         <v>95</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>43</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>42</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H10" s="21" t="s">
         <v>21</v>
@@ -2532,40 +2535,40 @@
         <v>22</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D11" s="21" t="s">
+      <c r="E11" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F11" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F11" s="21" t="s">
+      <c r="G11" s="21" t="s">
         <v>103</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>104</v>
       </c>
       <c r="H11" s="21" t="s">
         <v>99</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>100</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.3">
@@ -2573,19 +2576,19 @@
         <v>95</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D12" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>110</v>
-      </c>
       <c r="G12" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H12" s="21" t="s">
         <v>99</v>
@@ -2594,7 +2597,7 @@
         <v>94</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K12" s="1"/>
     </row>
@@ -2603,28 +2606,28 @@
         <v>95</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D13" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="H13" s="21" t="s">
         <v>114</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>115</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>94</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K13" s="1"/>
     </row>
@@ -2633,28 +2636,28 @@
         <v>19</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>40</v>
       </c>
       <c r="E14" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" s="21" t="s">
         <v>116</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>117</v>
       </c>
       <c r="G14" s="21" t="s">
         <v>48</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K14" s="1"/>
     </row>
@@ -2663,28 +2666,28 @@
         <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="F15" s="21" t="s">
         <v>120</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>121</v>
       </c>
       <c r="G15" s="21" t="s">
         <v>24</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K15" s="1"/>
     </row>
@@ -2693,13 +2696,13 @@
         <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D16" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="F16" s="21" t="s">
         <v>44</v>
@@ -2714,7 +2717,7 @@
         <v>22</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K16" s="1"/>
     </row>
@@ -2723,7 +2726,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>45</v>
@@ -2738,13 +2741,13 @@
         <v>29</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K17" s="1"/>
     </row>
@@ -2753,19 +2756,19 @@
         <v>49</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E18" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="F18" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="F18" s="21" t="s">
-        <v>182</v>
-      </c>
       <c r="G18" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H18" s="21" t="s">
         <v>50</v>
@@ -2774,7 +2777,7 @@
         <v>22</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K18" s="1"/>
     </row>
@@ -2783,19 +2786,19 @@
         <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D19" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="E19" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="E19" s="21" t="s">
-        <v>195</v>
-      </c>
       <c r="F19" s="21" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G19" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H19" s="21" t="s">
         <v>54</v>
@@ -2804,7 +2807,7 @@
         <v>22</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K19" s="1"/>
     </row>
@@ -2813,7 +2816,7 @@
         <v>52</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D20" s="21" t="s">
         <v>57</v>
@@ -2822,40 +2825,40 @@
         <v>35</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>56</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="2:11" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>88</v>
       </c>
       <c r="F21" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="G21" s="21" t="s">
         <v>196</v>
-      </c>
-      <c r="G21" s="21" t="s">
-        <v>199</v>
       </c>
       <c r="H21" s="21" t="s">
         <v>31</v>
@@ -2864,7 +2867,7 @@
         <v>22</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K21" s="1"/>
     </row>
@@ -2873,19 +2876,19 @@
         <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>89</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>23</v>
@@ -2894,7 +2897,7 @@
         <v>22</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K22" s="1"/>
     </row>
@@ -2903,10 +2906,10 @@
         <v>58</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E23" s="21" t="s">
         <v>55</v>
@@ -2915,16 +2918,16 @@
         <v>59</v>
       </c>
       <c r="G23" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="H23" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="H23" s="21" t="s">
-        <v>202</v>
-      </c>
       <c r="I23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K23" s="1"/>
     </row>
@@ -2933,10 +2936,10 @@
         <v>58</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E24" s="21" t="s">
         <v>55</v>
@@ -2945,25 +2948,25 @@
         <v>60</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="2:11" ht="99" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>41</v>
@@ -2984,7 +2987,7 @@
         <v>22</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K25" s="1"/>
     </row>
@@ -2993,7 +2996,7 @@
         <v>61</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D26" s="21" t="s">
         <v>62</v>
@@ -3014,7 +3017,7 @@
         <v>22</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K26" s="1"/>
     </row>
@@ -3023,7 +3026,7 @@
         <v>61</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D27" s="21" t="s">
         <v>67</v>
@@ -3035,37 +3038,37 @@
         <v>53</v>
       </c>
       <c r="G27" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="H27" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="H27" s="21" t="s">
-        <v>162</v>
-      </c>
       <c r="I27" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="2:11" ht="99" x14ac:dyDescent="0.3">
       <c r="B28" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E28" s="21" t="s">
         <v>170</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H28" s="21" t="s">
         <v>91</v>
@@ -3074,67 +3077,67 @@
         <v>22</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="2:11" ht="99" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>170</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G29" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="2:11" ht="99" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E30" s="21" t="s">
         <v>170</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G30" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="H30" s="21" t="s">
         <v>128</v>
-      </c>
-      <c r="H30" s="21" t="s">
-        <v>129</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>94</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K30" s="1"/>
     </row>
@@ -3143,19 +3146,19 @@
         <v>51</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D31" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="F31" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="F31" s="21" t="s">
+      <c r="G31" s="21" t="s">
         <v>156</v>
-      </c>
-      <c r="G31" s="21" t="s">
-        <v>157</v>
       </c>
       <c r="H31" s="21" t="s">
         <v>50</v>
@@ -3164,7 +3167,7 @@
         <v>22</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K31" s="1"/>
     </row>
@@ -3173,28 +3176,28 @@
         <v>70</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E32" s="21" t="s">
         <v>170</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K32" s="1"/>
     </row>
@@ -3203,7 +3206,7 @@
         <v>168</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D33" s="21" t="s">
         <v>169</v>
@@ -3221,42 +3224,42 @@
         <v>174</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>100</v>
+        <v>342</v>
       </c>
     </row>
     <row r="34" spans="2:11" ht="99" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E34" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="F34" s="21" t="s">
-        <v>132</v>
-      </c>
       <c r="G34" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H34" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="K34" s="1"/>
     </row>
@@ -3265,61 +3268,61 @@
         <v>71</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D35" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="G35" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="E35" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="F35" s="21" t="s">
+      <c r="H35" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="G35" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="H35" s="21" t="s">
-        <v>136</v>
-      </c>
       <c r="I35" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="K35" s="1"/>
     </row>
     <row r="36" spans="2:11" ht="99" x14ac:dyDescent="0.3">
       <c r="B36" s="21" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G36" s="21" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="H36" s="21" t="s">
         <v>174</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>100</v>
+        <v>344</v>
       </c>
     </row>
     <row r="37" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -3330,85 +3333,85 @@
         <v>38</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G37" s="21" t="s">
         <v>73</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K37" s="1"/>
     </row>
     <row r="38" spans="2:11" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G38" s="21" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="2:11" ht="66" x14ac:dyDescent="0.3">
       <c r="B39" s="21" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D39" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="G39" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="H39" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="E39" s="21" t="s">
-        <v>264</v>
-      </c>
-      <c r="F39" s="21" t="s">
-        <v>265</v>
-      </c>
-      <c r="G39" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="H39" s="21" t="s">
-        <v>266</v>
-      </c>
       <c r="I39" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J39" s="23" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K39" s="21"/>
     </row>
@@ -3417,28 +3420,28 @@
         <v>34</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F40" s="21" t="s">
         <v>35</v>
       </c>
       <c r="G40" s="21" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="I40" s="21" t="s">
         <v>175</v>
       </c>
       <c r="J40" s="23" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K40" s="21"/>
     </row>
@@ -3447,28 +3450,28 @@
         <v>34</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E41" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="F41" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="G41" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="F41" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="G41" s="21" t="s">
-        <v>211</v>
-      </c>
       <c r="H41" s="21" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="I41" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J41" s="23" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K41" s="21"/>
     </row>
@@ -3477,58 +3480,58 @@
         <v>34</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G42" s="21" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="I42" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J42" s="23" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K42" s="21"/>
     </row>
     <row r="43" spans="2:11" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B43" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D43" s="21" t="s">
         <v>36</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G43" s="21" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="I43" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J43" s="23" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K43" s="21"/>
     </row>
@@ -3543,22 +3546,22 @@
         <v>37</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G44" s="21" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I44" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J44" s="23" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="K44" s="21"/>
     </row>
@@ -3570,25 +3573,25 @@
         <v>75</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F45" s="22" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G45" s="21" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="I45" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J45" s="23" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="K45" s="21"/>
     </row>
@@ -3597,28 +3600,28 @@
         <v>93</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F46" s="22" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G46" s="21" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="I46" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J46" s="23" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K46" s="21"/>
     </row>
@@ -3627,31 +3630,31 @@
         <v>92</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D47" s="21" t="s">
+        <v>337</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="F47" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="G47" s="21" t="s">
+        <v>339</v>
+      </c>
+      <c r="H47" s="21" t="s">
         <v>340</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="I47" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="F47" s="22" t="s">
-        <v>341</v>
-      </c>
-      <c r="G47" s="21" t="s">
-        <v>342</v>
-      </c>
-      <c r="H47" s="21" t="s">
-        <v>343</v>
-      </c>
-      <c r="I47" s="21" t="s">
-        <v>176</v>
-      </c>
       <c r="J47" s="23" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K47" s="21" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="48" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
@@ -3662,310 +3665,310 @@
         <v>72</v>
       </c>
       <c r="D48" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="F48" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="G48" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="H48" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="E48" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="F48" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="G48" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="H48" s="21" t="s">
-        <v>226</v>
-      </c>
       <c r="I48" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J48" s="23" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="K48" s="21"/>
     </row>
     <row r="49" spans="2:11" ht="33" x14ac:dyDescent="0.3">
       <c r="B49" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D49" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="G49" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="H49" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="E49" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="F49" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="G49" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="H49" s="21" t="s">
-        <v>230</v>
-      </c>
       <c r="I49" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J49" s="23" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="K49" s="21"/>
     </row>
     <row r="50" spans="2:11" ht="33" x14ac:dyDescent="0.3">
       <c r="B50" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D50" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="E50" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F50" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="G50" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="H50" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="E50" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="F50" s="21" t="s">
-        <v>232</v>
-      </c>
-      <c r="G50" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="H50" s="21" t="s">
-        <v>234</v>
-      </c>
       <c r="I50" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J50" s="23" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="K50" s="21"/>
     </row>
     <row r="51" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B51" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="G51" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="H51" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="I51" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="J51" s="23" t="s">
         <v>329</v>
-      </c>
-      <c r="D51" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="E51" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="F51" s="21" t="s">
-        <v>236</v>
-      </c>
-      <c r="G51" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="H51" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="I51" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="J51" s="23" t="s">
-        <v>332</v>
       </c>
       <c r="K51" s="21"/>
     </row>
     <row r="52" spans="2:11" ht="33" x14ac:dyDescent="0.3">
       <c r="B52" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>76</v>
       </c>
       <c r="D52" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="G52" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="H52" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="E52" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="F52" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="G52" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="H52" s="21" t="s">
-        <v>242</v>
-      </c>
       <c r="I52" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J52" s="23" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="K52" s="21"/>
     </row>
     <row r="53" spans="2:11" ht="33" x14ac:dyDescent="0.3">
       <c r="B53" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>77</v>
       </c>
       <c r="D53" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="G53" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="H53" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="E53" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="F53" s="21" t="s">
-        <v>244</v>
-      </c>
-      <c r="G53" s="21" t="s">
-        <v>245</v>
-      </c>
-      <c r="H53" s="21" t="s">
-        <v>246</v>
-      </c>
       <c r="I53" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J53" s="23" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="K53" s="21"/>
     </row>
     <row r="54" spans="2:11" ht="66" x14ac:dyDescent="0.3">
       <c r="B54" s="21" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D54" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="G54" s="21" t="s">
         <v>277</v>
       </c>
-      <c r="E54" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="F54" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="G54" s="21" t="s">
-        <v>280</v>
-      </c>
       <c r="H54" s="21" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="I54" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J54" s="23" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="K54" s="21"/>
     </row>
     <row r="55" spans="2:11" ht="66" x14ac:dyDescent="0.3">
       <c r="B55" s="21" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>79</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E55" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="G55" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="F55" s="21" t="s">
+      <c r="H55" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="G55" s="21" t="s">
-        <v>285</v>
-      </c>
-      <c r="H55" s="21" t="s">
-        <v>286</v>
-      </c>
       <c r="I55" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J55" s="23" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="K55" s="21"/>
     </row>
     <row r="56" spans="2:11" ht="66" x14ac:dyDescent="0.3">
       <c r="B56" s="21" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D56" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="E56" s="21" t="s">
         <v>275</v>
       </c>
-      <c r="E56" s="21" t="s">
-        <v>278</v>
-      </c>
       <c r="F56" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="G56" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="H56" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="G56" s="21" t="s">
-        <v>280</v>
-      </c>
-      <c r="H56" s="21" t="s">
-        <v>287</v>
-      </c>
       <c r="I56" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J56" s="23" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="K56" s="21"/>
     </row>
     <row r="57" spans="2:11" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B57" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F57" s="21" t="s">
         <v>35</v>
       </c>
       <c r="G57" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H57" s="21" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="I57" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J57" s="23" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="K57" s="21"/>
     </row>
     <row r="58" spans="2:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>82</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E58" s="21" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F58" s="21" t="s">
         <v>53</v>
@@ -3980,67 +3983,67 @@
         <v>22</v>
       </c>
       <c r="J58" s="23" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="K58" s="21"/>
     </row>
     <row r="59" spans="2:11" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B59" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D59" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="G59" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="E59" s="21" t="s">
+      <c r="H59" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="F59" s="21" t="s">
-        <v>255</v>
-      </c>
-      <c r="G59" s="21" t="s">
-        <v>256</v>
-      </c>
-      <c r="H59" s="21" t="s">
-        <v>257</v>
-      </c>
       <c r="I59" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J59" s="23" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="K59" s="21"/>
     </row>
     <row r="60" spans="2:11" ht="99" x14ac:dyDescent="0.3">
       <c r="B60" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D60" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="G60" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="E60" s="21" t="s">
+      <c r="H60" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="F60" s="21" t="s">
-        <v>260</v>
-      </c>
-      <c r="G60" s="21" t="s">
-        <v>261</v>
-      </c>
-      <c r="H60" s="21" t="s">
-        <v>262</v>
-      </c>
       <c r="I60" s="21" t="s">
         <v>22</v>
       </c>
       <c r="J60" s="23" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="K60" s="21"/>
     </row>

</xml_diff>